<commit_message>
handling empty cells at the end of rows
</commit_message>
<xml_diff>
--- a/tests/data/test.xlsx
+++ b/tests/data/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -181,8 +181,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,9 +280,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -314,14 +310,11 @@
       <c r="B3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CSeite &amp;P</oddFooter>

</xml_diff>